<commit_message>
Delivery :Upload and autofill using existing documents
</commit_message>
<xml_diff>
--- a/assets/templates/Price_List.xlsx
+++ b/assets/templates/Price_List.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdallah_MTS\material_management_system\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdallah_MTS\material_management_system\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="826"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="Original Material" sheetId="23" r:id="rId1"/>
@@ -1338,8 +1338,8 @@
   </sheetPr>
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="D1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="1"/>

</xml_diff>